<commit_message>
docs: describe pivot table 1
</commit_message>
<xml_diff>
--- a/da/datasets/characters-popsda.xlsx
+++ b/da/datasets/characters-popsda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\movomo\Documents\200ok\da\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE54A63-DB30-41E0-BA22-771135E8C82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5579354B-25D0-4D59-A9F7-9BB0E8B96472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="4" r:id="rId1"/>
@@ -24,8 +24,8 @@
   </definedNames>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId5"/>
-    <pivotCache cacheId="43" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="19" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11536" uniqueCount="4073">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11538" uniqueCount="4075">
   <si>
     <t>id</t>
   </si>
@@ -12307,6 +12307,12 @@
   </si>
   <si>
     <t>Total Count of tier</t>
+  </si>
+  <si>
+    <t>동물 종 별, 성별 별로 캐릭터 티어 숫자의 평균을 낸 표입니다.</t>
+  </si>
+  <si>
+    <t>여자가 남자보다 평균적으로 높은 티어(낮은 숫자)에 있습니다.</t>
   </si>
 </sst>
 </file>
@@ -12406,64 +12412,6 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -12497,13 +12445,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -12511,6 +12452,71 @@
           <color auto="1"/>
         </top>
       </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -12705,7 +12711,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Seong Jun Yun" refreshedDate="44686.832318287037" backgroundQuery="1" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{86BDA8E3-D857-4629-B03D-304FEA7A95BC}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Seong Jun Yun" refreshedDate="44687.623282060187" backgroundQuery="1" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{86BDA8E3-D857-4629-B03D-304FEA7A95BC}">
   <cacheSource type="external" connectionId="2"/>
   <cacheFields count="5">
     <cacheField name="[Table1_2].[species].[species]" caption="species" numFmtId="0" hierarchy="6" level="1">
@@ -18695,7 +18701,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{508F7DE6-C2F7-4745-9E5C-07303BEA1D67}" name="PivotTable3" cacheId="43" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{508F7DE6-C2F7-4745-9E5C-07303BEA1D67}" name="PivotTable3" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G14" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" allDrilled="1" showAll="0" sortType="ascending" dataSourceSort="1" defaultAttributeDrillState="1">
@@ -18834,7 +18840,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A308747D-68C7-4330-BA4A-B3E99D123B59}" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A308747D-68C7-4330-BA4A-B3E99D123B59}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D40" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -18894,6 +18900,15 @@
         <item x="20"/>
         <item t="default"/>
       </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
     </pivotField>
     <pivotField showAll="0">
       <items count="7">
@@ -18928,76 +18943,88 @@
   </rowFields>
   <rowItems count="36">
     <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
       <x v="13"/>
     </i>
     <i>
       <x v="14"/>
     </i>
     <i>
-      <x v="15"/>
+      <x v="4"/>
     </i>
     <i>
-      <x v="16"/>
+      <x v="7"/>
     </i>
     <i>
-      <x v="17"/>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="23"/>
     </i>
     <i>
       <x v="18"/>
     </i>
     <i>
-      <x v="19"/>
+      <x v="5"/>
     </i>
     <i>
-      <x v="20"/>
+      <x v="9"/>
     </i>
     <i>
-      <x v="21"/>
+      <x v="2"/>
     </i>
     <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
+      <x v="15"/>
     </i>
     <i>
       <x v="24"/>
@@ -19006,31 +19033,19 @@
       <x v="25"/>
     </i>
     <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="31"/>
+      <x v="17"/>
     </i>
     <i>
       <x v="32"/>
     </i>
     <i>
-      <x v="33"/>
+      <x v="16"/>
     </i>
     <i>
-      <x v="34"/>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="3"/>
     </i>
     <i t="grand">
       <x/>
@@ -19094,17 +19109,17 @@
     <sortCondition ref="D1:D392"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{07BACF73-9115-4179-B3F5-16657E157D7D}" uniqueName="1" name="id" queryTableFieldId="1" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{91FF0001-5C9E-4EE9-B368-239AD32543A1}" uniqueName="2" name="name_ko" queryTableFieldId="2" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{DAB5CD76-81C2-43EB-B6AF-283F1D41DB7F}" uniqueName="3" name="name_en" queryTableFieldId="3" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{07BACF73-9115-4179-B3F5-16657E157D7D}" uniqueName="1" name="id" queryTableFieldId="1" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{91FF0001-5C9E-4EE9-B368-239AD32543A1}" uniqueName="2" name="name_ko" queryTableFieldId="2" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{DAB5CD76-81C2-43EB-B6AF-283F1D41DB7F}" uniqueName="3" name="name_en" queryTableFieldId="3" dataDxfId="11"/>
     <tableColumn id="4" xr3:uid="{A936419D-D481-46CB-9E6A-E2B64F662C61}" uniqueName="4" name="special" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{71FFDF28-3238-473B-86F9-4C46EE6AB020}" uniqueName="5" name="gender" queryTableFieldId="5" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{2EB2C359-E35B-4D1B-B82E-81DF3F74C401}" uniqueName="6" name="gender_asia" queryTableFieldId="6" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{494F9065-CD49-4AE9-A1DC-10851F82BD87}" uniqueName="7" name="species" queryTableFieldId="7" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{68F79698-FFFD-4C5B-AD10-1AB32DF4A7EB}" uniqueName="8" name="hobby" queryTableFieldId="8" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{01BA32B6-F7D5-41BF-A6CF-4D99E36049D7}" uniqueName="9" name="personality" queryTableFieldId="9" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{09344DAB-D35A-4CB9-A94F-36513A908DF8}" uniqueName="10" name="colors" queryTableFieldId="10" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{E7740184-597B-408F-A9E5-55CA74E27C36}" uniqueName="11" name="styles" queryTableFieldId="11" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{71FFDF28-3238-473B-86F9-4C46EE6AB020}" uniqueName="5" name="gender" queryTableFieldId="5" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{2EB2C359-E35B-4D1B-B82E-81DF3F74C401}" uniqueName="6" name="gender_asia" queryTableFieldId="6" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{494F9065-CD49-4AE9-A1DC-10851F82BD87}" uniqueName="7" name="species" queryTableFieldId="7" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{68F79698-FFFD-4C5B-AD10-1AB32DF4A7EB}" uniqueName="8" name="hobby" queryTableFieldId="8" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{01BA32B6-F7D5-41BF-A6CF-4D99E36049D7}" uniqueName="9" name="personality" queryTableFieldId="9" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{09344DAB-D35A-4CB9-A94F-36513A908DF8}" uniqueName="10" name="colors" queryTableFieldId="10" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{E7740184-597B-408F-A9E5-55CA74E27C36}" uniqueName="11" name="styles" queryTableFieldId="11" dataDxfId="4"/>
     <tableColumn id="12" xr3:uid="{683CA6C3-6469-4483-9D38-C6C3CEA5A5FA}" uniqueName="12" name="tier" queryTableFieldId="12"/>
     <tableColumn id="13" xr3:uid="{3C6A61F9-7520-4036-A931-207D83C44381}" uniqueName="13" name="rank" queryTableFieldId="13"/>
   </tableColumns>
@@ -19113,10 +19128,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1044E089-03B7-46A5-BD6B-5EA936428634}" name="Table1" displayName="Table1" ref="A1:X453" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="12" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1044E089-03B7-46A5-BD6B-5EA936428634}" name="Table1" displayName="Table1" ref="A1:X453" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="A1:X453" xr:uid="{1044E089-03B7-46A5-BD6B-5EA936428634}"/>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{144D981B-CE65-4C04-BD49-AFBEB2FB75BD}" name="id" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{144D981B-CE65-4C04-BD49-AFBEB2FB75BD}" name="id" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{06D8E56C-317D-455A-9C7D-10FC24EBF995}" name="name_ko"/>
     <tableColumn id="3" xr3:uid="{6A892FCB-7B0A-4FEF-94F2-72953542956A}" name="name_en"/>
     <tableColumn id="4" xr3:uid="{79E147C7-BE76-4CE7-9850-076C06E5BA1D}" name="special"/>
@@ -19432,7 +19447,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B5EDFD-9ADF-4BA9-A9F4-F33E11BE13E4}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19683,10 +19700,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F5CFAB-DA99-466D-9631-C159FCDDDE6D}">
-  <dimension ref="A3:D40"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19743,6 +19760,16 @@
     <col min="70" max="71" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4073</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4074</v>
+      </c>
+    </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>4067</v>
@@ -19767,486 +19794,486 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>377</v>
+        <v>2489</v>
       </c>
       <c r="B5" s="4">
-        <v>3.5714285714285716</v>
+        <v>1</v>
       </c>
       <c r="C5" s="4">
-        <v>4.666666666666667</v>
+        <v>2</v>
       </c>
       <c r="D5" s="4">
-        <v>4.1875</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>803</v>
+        <v>341</v>
       </c>
       <c r="B6" s="4">
-        <v>4.5999999999999996</v>
+        <v>2.75</v>
       </c>
       <c r="C6" s="4">
-        <v>5.2307692307692308</v>
+        <v>2.8333333333333335</v>
       </c>
       <c r="D6" s="4">
-        <v>5.0555555555555554</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>144</v>
+        <v>190</v>
       </c>
       <c r="B7" s="4">
-        <v>5.75</v>
+        <v>3.4285714285714284</v>
       </c>
       <c r="C7" s="4">
-        <v>5.333333333333333</v>
+        <v>3.4444444444444446</v>
       </c>
       <c r="D7" s="4">
-        <v>5.5714285714285712</v>
+        <v>3.4347826086956523</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>75</v>
+        <v>273</v>
       </c>
       <c r="B8" s="4">
-        <v>6</v>
+        <v>3.4</v>
       </c>
       <c r="C8" s="4">
-        <v>5.8571428571428568</v>
+        <v>3.5</v>
       </c>
       <c r="D8" s="4">
-        <v>5.8888888888888893</v>
+        <v>3.4545454545454546</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>190</v>
+        <v>365</v>
       </c>
       <c r="B9" s="4">
-        <v>3.4285714285714284</v>
+        <v>3.125</v>
       </c>
       <c r="C9" s="4">
-        <v>3.4444444444444446</v>
+        <v>5</v>
       </c>
       <c r="D9" s="4">
-        <v>3.4347826086956523</v>
+        <v>4.0625</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>389</v>
+        <v>518</v>
       </c>
       <c r="B10" s="4">
-        <v>5.333333333333333</v>
+        <v>4</v>
       </c>
       <c r="C10" s="4">
-        <v>5.4444444444444446</v>
+        <v>4.25</v>
       </c>
       <c r="D10" s="4">
-        <v>5.4</v>
+        <v>4.125</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>365</v>
+        <v>377</v>
       </c>
       <c r="B11" s="4">
-        <v>3.125</v>
+        <v>3.5714285714285716</v>
       </c>
       <c r="C11" s="4">
-        <v>5</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="D11" s="4">
-        <v>4.0625</v>
+        <v>4.1875</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>273</v>
+        <v>1907</v>
       </c>
       <c r="B12" s="4">
-        <v>3.4</v>
+        <v>4</v>
       </c>
       <c r="C12" s="4">
-        <v>3.5</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="D12" s="4">
-        <v>3.4545454545454546</v>
+        <v>4.333333333333333</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>45</v>
+        <v>248</v>
       </c>
       <c r="B13" s="4">
-        <v>4.5384615384615383</v>
+        <v>4</v>
       </c>
       <c r="C13" s="4">
-        <v>4</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D13" s="4">
-        <v>4.3888888888888893</v>
+        <v>4.375</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>297</v>
+        <v>45</v>
       </c>
       <c r="B14" s="4">
-        <v>5.75</v>
+        <v>4.5384615384615383</v>
       </c>
       <c r="C14" s="4">
-        <v>5.4</v>
+        <v>4</v>
       </c>
       <c r="D14" s="4">
-        <v>5.5555555555555554</v>
+        <v>4.3888888888888893</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="B15" s="4">
-        <v>5.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C15" s="4">
-        <v>5.1428571428571432</v>
+        <v>4.5</v>
       </c>
       <c r="D15" s="4">
-        <v>5.2222222222222223</v>
+        <v>4.4444444444444446</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>60</v>
+        <v>602</v>
       </c>
       <c r="B16" s="4">
-        <v>5.5714285714285712</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="C16" s="4">
-        <v>6</v>
+        <v>5.125</v>
       </c>
       <c r="D16" s="4">
-        <v>5.7857142857142856</v>
+        <v>4.6500000000000004</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>213</v>
+        <v>286</v>
       </c>
       <c r="B17" s="4">
-        <v>5.2857142857142856</v>
+        <v>5</v>
       </c>
       <c r="C17" s="4">
-        <v>5</v>
+        <v>4.625</v>
       </c>
       <c r="D17" s="4">
-        <v>5.1333333333333337</v>
+        <v>4.7692307692307692</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>2489</v>
+        <v>565</v>
       </c>
       <c r="B18" s="4">
-        <v>1</v>
+        <v>4.5714285714285712</v>
       </c>
       <c r="C18" s="4">
-        <v>2</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="D18" s="4">
-        <v>1.6666666666666667</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="B19" s="4">
-        <v>2.75</v>
+        <v>5.3</v>
       </c>
       <c r="C19" s="4">
-        <v>2.8333333333333335</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="D19" s="4">
-        <v>2.8</v>
+        <v>4.8461538461538458</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>746</v>
-      </c>
-      <c r="B20" s="4"/>
+        <v>507</v>
+      </c>
+      <c r="B20" s="4">
+        <v>4.9000000000000004</v>
+      </c>
       <c r="C20" s="4">
-        <v>5.5714285714285712</v>
+        <v>5.1428571428571432</v>
       </c>
       <c r="D20" s="4">
-        <v>5.5714285714285712</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>28</v>
+        <v>803</v>
       </c>
       <c r="B21" s="4">
-        <v>5.75</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C21" s="4">
-        <v>5.7777777777777777</v>
+        <v>5.2307692307692308</v>
       </c>
       <c r="D21" s="4">
-        <v>5.7692307692307692</v>
+        <v>5.0555555555555554</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B22" s="4"/>
+        <v>319</v>
+      </c>
+      <c r="B22" s="4">
+        <v>4.5999999999999996</v>
+      </c>
       <c r="C22" s="4">
-        <v>5.666666666666667</v>
+        <v>5.5</v>
       </c>
       <c r="D22" s="4">
-        <v>5.666666666666667</v>
+        <v>5.0909090909090908</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>88</v>
+        <v>213</v>
       </c>
       <c r="B23" s="4">
+        <v>5.2857142857142856</v>
+      </c>
+      <c r="C23" s="4">
         <v>5</v>
       </c>
-      <c r="C23" s="4">
-        <v>5.4</v>
-      </c>
       <c r="D23" s="4">
-        <v>5.2857142857142856</v>
+        <v>5.1333333333333337</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>2688</v>
+        <v>353</v>
       </c>
       <c r="B24" s="4">
-        <v>5.25</v>
-      </c>
-      <c r="C24" s="4"/>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="C24" s="4">
+        <v>5.75</v>
+      </c>
       <c r="D24" s="4">
-        <v>5.25</v>
+        <v>5.1428571428571432</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>330</v>
+        <v>130</v>
       </c>
       <c r="B25" s="4">
-        <v>5.3</v>
+        <v>5.5</v>
       </c>
       <c r="C25" s="4">
-        <v>3.3333333333333335</v>
+        <v>5.1428571428571432</v>
       </c>
       <c r="D25" s="4">
-        <v>4.8461538461538458</v>
+        <v>5.2222222222222223</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>518</v>
+        <v>2688</v>
       </c>
       <c r="B26" s="4">
-        <v>4</v>
-      </c>
-      <c r="C26" s="4">
-        <v>4.25</v>
-      </c>
+        <v>5.25</v>
+      </c>
+      <c r="C26" s="4"/>
       <c r="D26" s="4">
-        <v>4.125</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>507</v>
+        <v>1247</v>
       </c>
       <c r="B27" s="4">
-        <v>4.9000000000000004</v>
+        <v>5</v>
       </c>
       <c r="C27" s="4">
-        <v>5.1428571428571432</v>
+        <v>5.5</v>
       </c>
       <c r="D27" s="4">
-        <v>5</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>1247</v>
+        <v>88</v>
       </c>
       <c r="B28" s="4">
         <v>5</v>
       </c>
       <c r="C28" s="4">
-        <v>5.5</v>
+        <v>5.4</v>
       </c>
       <c r="D28" s="4">
-        <v>5.25</v>
+        <v>5.2857142857142856</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>179</v>
+        <v>389</v>
       </c>
       <c r="B29" s="4">
-        <v>5.5</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="C29" s="4">
-        <v>5.7142857142857144</v>
+        <v>5.4444444444444446</v>
       </c>
       <c r="D29" s="4">
-        <v>5.6</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>260</v>
+        <v>297</v>
       </c>
       <c r="B30" s="4">
-        <v>5.666666666666667</v>
+        <v>5.75</v>
       </c>
       <c r="C30" s="4">
-        <v>5.5</v>
+        <v>5.4</v>
       </c>
       <c r="D30" s="4">
-        <v>5.625</v>
+        <v>5.5555555555555554</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>319</v>
+        <v>144</v>
       </c>
       <c r="B31" s="4">
-        <v>4.5999999999999996</v>
+        <v>5.75</v>
       </c>
       <c r="C31" s="4">
-        <v>5.5</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="D31" s="4">
-        <v>5.0909090909090908</v>
+        <v>5.5714285714285712</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>1907</v>
-      </c>
-      <c r="B32" s="4">
-        <v>4</v>
-      </c>
+        <v>746</v>
+      </c>
+      <c r="B32" s="4"/>
       <c r="C32" s="4">
-        <v>4.666666666666667</v>
+        <v>5.5714285714285712</v>
       </c>
       <c r="D32" s="4">
-        <v>4.333333333333333</v>
+        <v>5.5714285714285712</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>101</v>
+        <v>179</v>
       </c>
       <c r="B33" s="4">
-        <v>4.4000000000000004</v>
+        <v>5.5</v>
       </c>
       <c r="C33" s="4">
-        <v>4.5</v>
+        <v>5.7142857142857144</v>
       </c>
       <c r="D33" s="4">
-        <v>4.4444444444444446</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>565</v>
+        <v>260</v>
       </c>
       <c r="B34" s="4">
-        <v>4.5714285714285712</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="C34" s="4">
-        <v>5.333333333333333</v>
+        <v>5.5</v>
       </c>
       <c r="D34" s="4">
-        <v>4.8</v>
+        <v>5.625</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>602</v>
-      </c>
-      <c r="B35" s="4">
-        <v>4.333333333333333</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="B35" s="4"/>
       <c r="C35" s="4">
-        <v>5.125</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="D35" s="4">
-        <v>4.6500000000000004</v>
+        <v>5.666666666666667</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>286</v>
+        <v>455</v>
       </c>
       <c r="B36" s="4">
-        <v>5</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="C36" s="4">
-        <v>4.625</v>
+        <v>5.75</v>
       </c>
       <c r="D36" s="4">
-        <v>4.7692307692307692</v>
+        <v>5.7142857142857144</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>455</v>
+        <v>28</v>
       </c>
       <c r="B37" s="4">
-        <v>5.666666666666667</v>
+        <v>5.75</v>
       </c>
       <c r="C37" s="4">
-        <v>5.75</v>
+        <v>5.7777777777777777</v>
       </c>
       <c r="D37" s="4">
-        <v>5.7142857142857144</v>
+        <v>5.7692307692307692</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>248</v>
+        <v>60</v>
       </c>
       <c r="B38" s="4">
-        <v>4</v>
+        <v>5.5714285714285712</v>
       </c>
       <c r="C38" s="4">
-        <v>4.5999999999999996</v>
+        <v>6</v>
       </c>
       <c r="D38" s="4">
-        <v>4.375</v>
+        <v>5.7857142857142856</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>353</v>
+        <v>75</v>
       </c>
       <c r="B39" s="4">
-        <v>4.333333333333333</v>
+        <v>6</v>
       </c>
       <c r="C39" s="4">
-        <v>5.75</v>
+        <v>5.8571428571428568</v>
       </c>
       <c r="D39" s="4">
-        <v>5.1428571428571432</v>
+        <v>5.8888888888888893</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>